<commit_message>
Improved multi-model single output herd prob
</commit_message>
<xml_diff>
--- a/data/goat_results.xlsx
+++ b/data/goat_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\NYSDAM\small ruminant johnes RESEARCH\goat stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\STAT385 and Cornell\johne\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D285D658-4B86-4136-A697-CC3B66E7E316}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D1A449-5642-443B-B23C-C60B45BB6939}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14250" yWindow="0" windowWidth="14325" windowHeight="14205" activeTab="2" xr2:uid="{9152E247-4AD0-40D4-BDF8-4206309FB6ED}"/>
+    <workbookView xWindow="14250" yWindow="0" windowWidth="14325" windowHeight="14205" activeTab="1" xr2:uid="{9152E247-4AD0-40D4-BDF8-4206309FB6ED}"/>
   </bookViews>
   <sheets>
     <sheet name="pivot table" sheetId="2" r:id="rId1"/>
@@ -19,26 +19,18 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2114" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="148">
   <si>
     <t>breed</t>
   </si>
@@ -480,6 +472,9 @@
   <si>
     <t>sample number</t>
   </si>
+  <si>
+    <t>farm_num</t>
+  </si>
 </sst>
 </file>
 
@@ -767,7 +762,71 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -794,7 +853,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[goat results NO ID.xlsx]pivot table!PivotTable2</c:name>
+    <c:name>[goat_results.xlsx]pivot table!PivotTable2</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -1374,47 +1433,6 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="11"/>
@@ -1430,47 +1448,6 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="12"/>
@@ -1486,47 +1463,6 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="13"/>
@@ -1542,47 +1478,6 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="14"/>
@@ -1598,47 +1493,6 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="15"/>
@@ -1654,47 +1508,6 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -3739,85 +3552,85 @@
               <c:strCache>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>T</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>W</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>O</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>A1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>U</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>V</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>L</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>M</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>J</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Y</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>A</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="18">
                   <c:v>B</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>C</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="19">
+                  <c:v>Z</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>D</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>E</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="23">
+                  <c:v>N</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>R</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>F</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>G</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>H</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>I</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>J</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>K</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>L</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>M</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>N</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>O</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>P</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Q</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>R</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>S</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>T</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>U</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>V</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>W</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>X</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Y</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Z</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>A1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3829,85 +3642,85 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="17">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="19">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="21">
                   <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3948,85 +3761,85 @@
               <c:strCache>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>T</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>W</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>O</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>A1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>U</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>V</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>L</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>M</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>J</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Y</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>A</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="18">
                   <c:v>B</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>C</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="19">
+                  <c:v>Z</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>D</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>E</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="23">
+                  <c:v>N</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>R</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>F</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>G</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>H</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>I</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>J</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>K</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>L</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>M</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>N</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>O</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>P</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Q</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>R</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>S</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>T</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>U</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>V</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>W</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>X</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Y</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Z</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>A1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4038,40 +3851,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="19">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="21">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="23">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="26">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4112,85 +3925,85 @@
               <c:strCache>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>T</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>W</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>O</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>A1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>U</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>V</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>L</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>M</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>J</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Y</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>A</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="18">
                   <c:v>B</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>C</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="19">
+                  <c:v>Z</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>D</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>E</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="23">
+                  <c:v>N</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>R</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>F</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>G</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>H</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>I</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>J</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>K</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>L</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>M</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>N</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>O</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>P</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Q</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>R</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>S</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>T</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>U</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>V</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>W</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>X</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Y</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Z</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>A1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4202,85 +4015,85 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="17">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="19">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="21">
                   <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>20</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4321,85 +4134,85 @@
               <c:strCache>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>T</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>W</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>O</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>A1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>U</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>V</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>L</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>M</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>J</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Y</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>A</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="18">
                   <c:v>B</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>C</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="19">
+                  <c:v>Z</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>D</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>E</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="23">
+                  <c:v>N</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>R</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>F</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>G</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>H</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>I</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>J</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>K</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>L</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>M</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>N</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>O</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>P</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Q</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>R</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>S</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>T</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>U</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>V</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>W</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>X</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Y</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Z</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>A1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4410,17 +4223,17 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
-                <c:pt idx="15">
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4461,85 +4274,85 @@
               <c:strCache>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>T</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>W</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>O</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>A1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>U</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>V</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>L</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>M</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>J</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Y</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>A</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="18">
                   <c:v>B</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>C</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="19">
+                  <c:v>Z</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>D</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>E</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="23">
+                  <c:v>N</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>R</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>F</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>G</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>H</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>I</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>J</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>K</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>L</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>M</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>N</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>O</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>P</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Q</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>R</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>S</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>T</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>U</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>V</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>W</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>X</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Y</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Z</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>A1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4551,85 +4364,85 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="17">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="19">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="21">
                   <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>20</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4670,85 +4483,85 @@
               <c:strCache>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>T</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>W</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>O</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>A1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>U</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>V</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>L</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>M</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>J</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Y</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>A</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="18">
                   <c:v>B</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>C</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="19">
+                  <c:v>Z</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>D</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>E</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="23">
+                  <c:v>N</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>R</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>F</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>G</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>H</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>I</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>J</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>K</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>L</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>M</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>N</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>O</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>P</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Q</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>R</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>S</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>T</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>U</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>V</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>W</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>X</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Y</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Z</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>A1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4759,7 +4572,7 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
-                <c:pt idx="14">
+                <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -4803,85 +4616,85 @@
               <c:strCache>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
+                  <c:v>T</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>W</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>O</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>A1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>X</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>E</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>U</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>V</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>L</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>G</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>M</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>K</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>J</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Q</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Y</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>A</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="18">
                   <c:v>B</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>C</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="19">
+                  <c:v>Z</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>I</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>P</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>D</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>E</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="23">
+                  <c:v>N</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>H</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>R</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>F</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>G</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>H</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>I</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>J</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>K</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>L</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>M</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>N</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>O</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>P</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Q</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>R</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>S</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>T</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>U</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>V</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>W</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>X</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Y</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Z</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>A1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4892,22 +4705,22 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
-                <c:pt idx="5">
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="26">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -12330,7 +12143,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{755DB0BC-F359-49D9-AF1C-0ED16552B934}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{755DB0BC-F359-49D9-AF1C-0ED16552B934}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:I33" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField dataField="1" showAll="0">
@@ -12666,6 +12479,27 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9055CF3-6865-4531-AF3B-0EE86E82ABF0}" name="Table1" displayName="Table1" ref="B37:J64" totalsRowShown="0" tableBorderDxfId="6">
+  <autoFilter ref="B37:J64" xr:uid="{ECC8710C-9C1F-4703-A028-E4CE81E38AEC}"/>
+  <sortState ref="B38:J64">
+    <sortCondition ref="B37:B64"/>
+  </sortState>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{96452084-1C47-43AF-8F64-F77D8D09DC4D}" name="farm_num" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{9A53AFCE-BF98-4EB7-A53A-DB1470D61C48}" name="farm" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{E912CAE7-2DB6-4AFA-8476-C9BBFBC72E31}" name="elisa Neg" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{20C0DBE1-98F8-4B28-A3E3-AB68077992BB}" name="ELISA pos" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{08E7F8F7-E5CC-4051-88A4-D79D95F119D4}" name="PCR neg" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{6ABC44E5-E2F1-4541-9A5B-B2DB5D04B2EA}" name="PCR pos"/>
+    <tableColumn id="7" xr3:uid="{1B377E33-C728-46F5-AF88-A3B328D999DB}" name="Culture Neg" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{6462EF35-460A-4213-B4E6-47DAD252B8D3}" name="Culture inconclusive"/>
+    <tableColumn id="9" xr3:uid="{298A7E51-88BC-431D-895D-1E464159A5BD}" name="Culture positive"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -12965,7 +12799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5B8AC7-3416-4E3B-8CCE-1B7D9C1653FC}">
   <dimension ref="A3:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="I6" sqref="I6:I32"/>
     </sheetView>
   </sheetViews>
@@ -13662,13 +13496,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C855680-FFC7-47D5-9C6A-305B625E0187}">
   <dimension ref="A2:N65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9:L26"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="9.140625" style="31"/>
+    <col min="2" max="2" width="12.28515625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="31"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14733,8 +14575,11 @@
         <v>318</v>
       </c>
     </row>
-    <row r="36" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="31" t="s">
+        <v>147</v>
+      </c>
       <c r="C37" s="31" t="s">
         <v>134</v>
       </c>
@@ -14756,541 +14601,622 @@
       <c r="I37" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="J37" s="42" t="s">
+      <c r="J37" s="41" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C38" s="35" t="s">
-        <v>109</v>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="35">
+        <v>1</v>
+      </c>
+      <c r="C38" s="52" t="s">
+        <v>127</v>
       </c>
       <c r="D38" s="43">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E38" s="44"/>
       <c r="F38" s="43">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G38" s="44"/>
       <c r="H38" s="43">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="I38" s="44"/>
-      <c r="J38" s="45"/>
-    </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C39" s="35" t="s">
-        <v>110</v>
+      <c r="J38" s="44"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="35">
+        <v>2</v>
+      </c>
+      <c r="C39" s="52" t="s">
+        <v>118</v>
       </c>
       <c r="D39" s="43">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E39" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" s="43">
-        <v>20</v>
-      </c>
-      <c r="G39" s="44"/>
+        <v>13</v>
+      </c>
+      <c r="G39" s="49">
+        <v>1</v>
+      </c>
       <c r="H39" s="43">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I39" s="44"/>
-      <c r="J39" s="45"/>
-    </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C40" s="35" t="s">
-        <v>111</v>
+      <c r="J39" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="35">
+        <v>3</v>
+      </c>
+      <c r="C40" s="52" t="s">
+        <v>124</v>
       </c>
       <c r="D40" s="43">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E40" s="44"/>
       <c r="F40" s="43">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G40" s="44"/>
       <c r="H40" s="43">
-        <v>11</v>
-      </c>
-      <c r="I40" s="44"/>
-      <c r="J40" s="45"/>
-    </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="I40" s="44">
+        <v>1</v>
+      </c>
+      <c r="J40" s="44"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="35">
+        <v>4</v>
+      </c>
       <c r="C41" s="52" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="D41" s="43">
-        <v>13</v>
-      </c>
-      <c r="E41" s="44"/>
+        <v>6</v>
+      </c>
+      <c r="E41" s="49">
+        <v>1</v>
+      </c>
       <c r="F41" s="43">
-        <v>13</v>
-      </c>
-      <c r="G41" s="44"/>
+        <v>7</v>
+      </c>
+      <c r="G41" s="50">
+        <v>0</v>
+      </c>
       <c r="H41" s="43">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I41" s="44"/>
-      <c r="J41" s="45"/>
-    </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J41" s="44"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="35">
+        <v>5</v>
+      </c>
       <c r="C42" s="52" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="D42" s="43">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E42" s="44"/>
       <c r="F42" s="43">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G42" s="44"/>
       <c r="H42" s="43">
+        <v>5</v>
+      </c>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="35">
         <v>6</v>
       </c>
-      <c r="I42" s="44"/>
-      <c r="J42" s="45"/>
-    </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C43" s="52" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
       <c r="D43" s="43">
-        <v>8</v>
-      </c>
-      <c r="E43" s="49">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E43" s="44"/>
       <c r="F43" s="43">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G43" s="44"/>
       <c r="H43" s="43">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I43" s="44"/>
-      <c r="J43" s="51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J43" s="44"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="35">
+        <v>7</v>
+      </c>
       <c r="C44" s="52" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D44" s="43">
-        <v>19</v>
-      </c>
-      <c r="E44" s="49">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E44" s="44"/>
       <c r="F44" s="43">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="G44" s="44"/>
       <c r="H44" s="43">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="I44" s="44"/>
-      <c r="J44" s="45"/>
-    </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J44" s="44"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="35">
+        <v>8</v>
+      </c>
       <c r="C45" s="52" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="D45" s="43">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E45" s="44"/>
       <c r="F45" s="43">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G45" s="44"/>
       <c r="H45" s="43">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I45" s="44"/>
-      <c r="J45" s="45"/>
-    </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J45" s="44"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="35">
+        <v>9</v>
+      </c>
       <c r="C46" s="52" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="D46" s="43">
-        <v>11</v>
-      </c>
-      <c r="E46" s="44"/>
+        <v>10</v>
+      </c>
+      <c r="E46" s="49">
+        <v>1</v>
+      </c>
       <c r="F46" s="43">
-        <v>11</v>
-      </c>
-      <c r="G46" s="44"/>
+        <v>10</v>
+      </c>
+      <c r="G46" s="49">
+        <v>1</v>
+      </c>
       <c r="H46" s="43">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I46" s="44"/>
-      <c r="J46" s="45"/>
-    </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J46" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="35">
+        <v>10</v>
+      </c>
       <c r="C47" s="52" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D47" s="43">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E47" s="44"/>
       <c r="F47" s="43">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G47" s="44"/>
       <c r="H47" s="43">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I47" s="44"/>
-      <c r="J47" s="45"/>
-    </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J47" s="44"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="35">
+        <v>11</v>
+      </c>
       <c r="C48" s="52" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D48" s="43">
-        <v>6</v>
-      </c>
-      <c r="E48" s="44"/>
+        <v>19</v>
+      </c>
+      <c r="E48" s="49">
+        <v>1</v>
+      </c>
       <c r="F48" s="43">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="G48" s="44"/>
       <c r="H48" s="43">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="I48" s="44"/>
-      <c r="J48" s="45"/>
-    </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J48" s="44"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49" s="35">
+        <v>12</v>
+      </c>
       <c r="C49" s="52" t="s">
-        <v>122</v>
+        <v>22</v>
       </c>
       <c r="D49" s="43">
-        <v>7</v>
-      </c>
-      <c r="E49" s="44"/>
+        <v>16</v>
+      </c>
+      <c r="E49" s="49">
+        <v>2</v>
+      </c>
       <c r="F49" s="43">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="G49" s="44"/>
       <c r="H49" s="43">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I49" s="44"/>
-      <c r="J49" s="45"/>
-    </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J49" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" s="35">
+        <v>13</v>
+      </c>
       <c r="C50" s="52" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
       <c r="D50" s="43">
-        <v>16</v>
-      </c>
-      <c r="E50" s="49">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E50" s="44"/>
       <c r="F50" s="43">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="G50" s="44"/>
       <c r="H50" s="43">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="I50" s="44"/>
-      <c r="J50" s="51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J50" s="44"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="35">
+        <v>14</v>
+      </c>
       <c r="C51" s="52" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D51" s="43">
-        <v>6</v>
-      </c>
-      <c r="E51" s="49">
-        <v>3</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E51" s="44"/>
       <c r="F51" s="43">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G51" s="44"/>
       <c r="H51" s="43">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I51" s="44"/>
-      <c r="J51" s="45"/>
-    </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J51" s="44"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="35">
+        <v>15</v>
+      </c>
       <c r="C52" s="52" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D52" s="43">
-        <v>13</v>
-      </c>
-      <c r="E52" s="44"/>
+        <v>16</v>
+      </c>
+      <c r="E52" s="49">
+        <v>4</v>
+      </c>
       <c r="F52" s="43">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G52" s="44"/>
       <c r="H52" s="43">
-        <v>12</v>
-      </c>
-      <c r="I52" s="44">
+        <v>19</v>
+      </c>
+      <c r="I52" s="44"/>
+      <c r="J52" s="49">
         <v>1</v>
       </c>
-      <c r="J52" s="45"/>
-    </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="35">
+        <v>16</v>
+      </c>
       <c r="C53" s="52" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D53" s="43">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E53" s="49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" s="43">
-        <v>19</v>
-      </c>
-      <c r="G53" s="49">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G53" s="44"/>
       <c r="H53" s="43">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I53" s="44"/>
-      <c r="J53" s="51">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C54" s="52" t="s">
-        <v>126</v>
+      <c r="J53" s="44"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B54" s="35">
+        <v>17</v>
+      </c>
+      <c r="C54" s="35" t="s">
+        <v>111</v>
       </c>
       <c r="D54" s="43">
-        <v>16</v>
-      </c>
-      <c r="E54" s="49">
-        <v>4</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E54" s="44"/>
       <c r="F54" s="43">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G54" s="44"/>
       <c r="H54" s="43">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="I54" s="44"/>
-      <c r="J54" s="51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C55" s="52" t="s">
-        <v>116</v>
+      <c r="J54" s="44"/>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B55" s="35">
+        <v>18</v>
+      </c>
+      <c r="C55" s="35" t="s">
+        <v>109</v>
       </c>
       <c r="D55" s="43">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E55" s="44"/>
       <c r="F55" s="43">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G55" s="44"/>
       <c r="H55" s="43">
+        <v>11</v>
+      </c>
+      <c r="I55" s="44"/>
+      <c r="J55" s="44"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B56" s="35">
         <v>19</v>
       </c>
-      <c r="I55" s="44"/>
-      <c r="J55" s="45"/>
-    </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C56" s="52" t="s">
-        <v>117</v>
+      <c r="C56" s="35" t="s">
+        <v>110</v>
       </c>
       <c r="D56" s="43">
-        <v>4</v>
-      </c>
-      <c r="E56" s="44"/>
+        <v>18</v>
+      </c>
+      <c r="E56" s="49">
+        <v>2</v>
+      </c>
       <c r="F56" s="43">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G56" s="44"/>
       <c r="H56" s="43">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="I56" s="44"/>
-      <c r="J56" s="45"/>
-    </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J56" s="44"/>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="35">
+        <v>20</v>
+      </c>
       <c r="C57" s="52" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D57" s="43">
-        <v>20</v>
-      </c>
-      <c r="E57" s="44"/>
+        <v>8</v>
+      </c>
+      <c r="E57" s="49">
+        <v>1</v>
+      </c>
       <c r="F57" s="43">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G57" s="44"/>
       <c r="H57" s="43">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I57" s="44"/>
-      <c r="J57" s="45"/>
-    </row>
-    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J57" s="44"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="35">
+        <v>21</v>
+      </c>
       <c r="C58" s="52" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D58" s="43">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E58" s="44"/>
       <c r="F58" s="43">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G58" s="44"/>
       <c r="H58" s="43">
+        <v>11</v>
+      </c>
+      <c r="I58" s="44"/>
+      <c r="J58" s="44"/>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B59" s="35">
+        <v>22</v>
+      </c>
+      <c r="C59" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="D59" s="43">
+        <v>18</v>
+      </c>
+      <c r="E59" s="49">
         <v>2</v>
       </c>
-      <c r="I58" s="44"/>
-      <c r="J58" s="45"/>
-    </row>
-    <row r="59" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C59" s="52" t="s">
-        <v>129</v>
-      </c>
-      <c r="D59" s="43">
-        <v>10</v>
-      </c>
-      <c r="E59" s="49">
-        <v>1</v>
-      </c>
       <c r="F59" s="43">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G59" s="49">
         <v>1</v>
       </c>
       <c r="H59" s="43">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I59" s="44"/>
-      <c r="J59" s="51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J59" s="49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="35">
+        <v>23</v>
+      </c>
       <c r="C60" s="52" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D60" s="43">
         <v>13</v>
       </c>
-      <c r="E60" s="49">
-        <v>1</v>
-      </c>
+      <c r="E60" s="44"/>
       <c r="F60" s="43">
         <v>13</v>
       </c>
-      <c r="G60" s="49">
-        <v>1</v>
-      </c>
+      <c r="G60" s="44"/>
       <c r="H60" s="43">
         <v>13</v>
       </c>
       <c r="I60" s="44"/>
-      <c r="J60" s="51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J60" s="44"/>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B61" s="35">
+        <v>24</v>
+      </c>
       <c r="C61" s="52" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D61" s="43">
-        <v>5</v>
-      </c>
-      <c r="E61" s="44"/>
+        <v>6</v>
+      </c>
+      <c r="E61" s="49">
+        <v>3</v>
+      </c>
       <c r="F61" s="43">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G61" s="44"/>
       <c r="H61" s="43">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I61" s="44"/>
-      <c r="J61" s="45"/>
-    </row>
-    <row r="62" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J61" s="44"/>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B62" s="35">
+        <v>25</v>
+      </c>
       <c r="C62" s="52" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="D62" s="43">
-        <v>19</v>
-      </c>
-      <c r="E62" s="49">
-        <v>1</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E62" s="44"/>
       <c r="F62" s="43">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="G62" s="44"/>
       <c r="H62" s="43">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="I62" s="44"/>
-      <c r="J62" s="45"/>
-    </row>
-    <row r="63" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J62" s="44"/>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B63" s="35">
+        <v>26</v>
+      </c>
       <c r="C63" s="52" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="D63" s="43">
-        <v>8</v>
-      </c>
-      <c r="E63" s="49">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E63" s="44"/>
       <c r="F63" s="43">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="G63" s="44"/>
       <c r="H63" s="43">
+        <v>19</v>
+      </c>
+      <c r="I63" s="44"/>
+      <c r="J63" s="44"/>
+    </row>
+    <row r="64" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="35">
+        <v>27</v>
+      </c>
+      <c r="C64" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="I63" s="44"/>
-      <c r="J63" s="45"/>
-    </row>
-    <row r="64" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C64" s="52" t="s">
-        <v>133</v>
-      </c>
       <c r="D64" s="43">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E64" s="49">
+        <v>2</v>
+      </c>
+      <c r="F64" s="43">
+        <v>10</v>
+      </c>
+      <c r="G64" s="44"/>
+      <c r="H64" s="43">
+        <v>9</v>
+      </c>
+      <c r="I64" s="44"/>
+      <c r="J64" s="49">
         <v>1</v>
       </c>
-      <c r="F64" s="43">
-        <v>7</v>
-      </c>
-      <c r="G64" s="50">
-        <v>0</v>
-      </c>
-      <c r="H64" s="43">
-        <v>7</v>
-      </c>
-      <c r="I64" s="44"/>
-      <c r="J64" s="45"/>
     </row>
     <row r="65" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C65" s="46"/>
@@ -15305,6 +15231,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -15312,7 +15241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8980B8D-CFA7-43C4-A511-C30E87FC160D}">
   <dimension ref="A1:AM320"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
@@ -27252,7 +27181,7 @@
       <c r="J320" s="32"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AM319">
+  <sortState ref="A2:AM319">
     <sortCondition ref="A2:A319"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>